<commit_message>
Update table and summary for literature review
</commit_message>
<xml_diff>
--- a/Sunny/Literature reading table.xlsx
+++ b/Sunny/Literature reading table.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gosun\Desktop\2023 S1\COMPSYS 700A_B\webApp\P4P_-26\Sunny\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gosun\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9B463680-105F-4653-973E-6EC85CF1C260}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92D99860-DDD2-4327-B5A9-CA8724F53ADE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="20186" windowHeight="12800" xr2:uid="{26EFEBA5-DBB9-4615-9FED-72CE28BB6DDB}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="137">
   <si>
     <t>2023 P4P Literature Review Readings</t>
   </si>
@@ -458,6 +458,15 @@
   </si>
   <si>
     <t>Annotation and processing of continuous emotional attributes: Challenges and opportunities</t>
+  </si>
+  <si>
+    <t>Data modality</t>
+  </si>
+  <si>
+    <t>multi (speech, video)</t>
+  </si>
+  <si>
+    <t>multi</t>
   </si>
 </sst>
 </file>
@@ -531,12 +540,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="4">
@@ -587,7 +602,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -623,24 +638,34 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -959,10 +984,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51385E3E-ECF8-4CD1-B57E-B22F63BA8D25}">
-  <dimension ref="A2:K33"/>
+  <dimension ref="A2:L33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="84" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -978,12 +1003,12 @@
     <col min="11" max="11" width="19.8203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.5">
       <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.5">
       <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
@@ -1014,15 +1039,20 @@
       <c r="K3" s="3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" ht="71.7" x14ac:dyDescent="0.5">
+      <c r="L3" s="22" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="71.7" x14ac:dyDescent="0.5">
       <c r="A4">
         <v>1</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="2"/>
+      <c r="C4" s="2">
+        <v>2022</v>
+      </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2" t="s">
         <v>8</v>
@@ -1045,15 +1075,20 @@
       <c r="K4" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" ht="71.7" x14ac:dyDescent="0.5">
+      <c r="L4" s="23" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="71.7" x14ac:dyDescent="0.5">
       <c r="A5">
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="1"/>
+      <c r="C5" s="1">
+        <v>2021</v>
+      </c>
       <c r="D5" s="5" t="s">
         <v>19</v>
       </c>
@@ -1068,15 +1103,20 @@
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
-    </row>
-    <row r="6" spans="1:11" ht="43" x14ac:dyDescent="0.5">
+      <c r="L5" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="43" x14ac:dyDescent="0.5">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="1"/>
+      <c r="C6" s="1">
+        <v>2007</v>
+      </c>
       <c r="D6" s="4" t="s">
         <v>22</v>
       </c>
@@ -1092,7 +1132,7 @@
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
     </row>
-    <row r="7" spans="1:11" ht="143.35" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:12" ht="143.35" x14ac:dyDescent="0.5">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1115,7 +1155,7 @@
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
     </row>
-    <row r="8" spans="1:11" ht="100.35" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:12" ht="100.35" x14ac:dyDescent="0.5">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1140,7 +1180,7 @@
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
     </row>
-    <row r="9" spans="1:11" ht="57.35" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:12" ht="57.35" x14ac:dyDescent="0.5">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1161,7 +1201,7 @@
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
     </row>
-    <row r="10" spans="1:11" ht="100.35" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:12" ht="100.35" x14ac:dyDescent="0.5">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1186,11 +1226,11 @@
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
     </row>
-    <row r="11" spans="1:11" ht="172" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:12" ht="172" x14ac:dyDescent="0.5">
       <c r="A11">
         <v>9</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="21" t="s">
         <v>41</v>
       </c>
       <c r="C11" s="2">
@@ -1215,7 +1255,7 @@
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
     </row>
-    <row r="12" spans="1:11" ht="129" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:12" ht="129" x14ac:dyDescent="0.5">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1240,11 +1280,11 @@
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
     </row>
-    <row r="13" spans="1:11" ht="71.7" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:12" ht="71.7" x14ac:dyDescent="0.5">
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="18" t="s">
         <v>46</v>
       </c>
       <c r="C13" s="2">
@@ -1271,7 +1311,7 @@
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
     </row>
-    <row r="14" spans="1:11" ht="71.7" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:12" ht="71.7" x14ac:dyDescent="0.5">
       <c r="A14">
         <v>11</v>
       </c>
@@ -1300,11 +1340,11 @@
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
     </row>
-    <row r="15" spans="1:11" ht="129" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:12" ht="129" x14ac:dyDescent="0.5">
       <c r="A15">
         <v>13</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="21" t="s">
         <v>55</v>
       </c>
       <c r="C15" s="2">
@@ -1329,7 +1369,7 @@
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
     </row>
-    <row r="16" spans="1:11" ht="86" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:12" ht="86" x14ac:dyDescent="0.5">
       <c r="A16">
         <v>14</v>
       </c>
@@ -1358,7 +1398,7 @@
       <c r="A17">
         <v>15</v>
       </c>
-      <c r="B17" s="9" t="s">
+      <c r="B17" s="18" t="s">
         <v>74</v>
       </c>
       <c r="C17" s="2">
@@ -1383,7 +1423,7 @@
       <c r="A18">
         <v>16</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="21" t="s">
         <v>67</v>
       </c>
       <c r="C18" s="2">
@@ -1489,7 +1529,7 @@
       <c r="A22">
         <v>20</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="21" t="s">
         <v>96</v>
       </c>
       <c r="C22" s="2">
@@ -1539,7 +1579,7 @@
       <c r="A24">
         <v>22</v>
       </c>
-      <c r="B24" s="9" t="s">
+      <c r="B24" s="18" t="s">
         <v>103</v>
       </c>
       <c r="C24" s="2">
@@ -1572,7 +1612,7 @@
       <c r="A25">
         <v>23</v>
       </c>
-      <c r="B25" s="13" t="s">
+      <c r="B25" s="17" t="s">
         <v>110</v>
       </c>
       <c r="C25" s="2">
@@ -1593,7 +1633,7 @@
       <c r="A26">
         <v>24</v>
       </c>
-      <c r="B26" s="9" t="s">
+      <c r="B26" s="18" t="s">
         <v>112</v>
       </c>
       <c r="C26" s="2">
@@ -1602,10 +1642,10 @@
       <c r="D26" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="E26" s="14" t="s">
+      <c r="E26" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="F26" s="14" t="s">
+      <c r="F26" s="13" t="s">
         <v>116</v>
       </c>
       <c r="G26" s="2"/>
@@ -1620,7 +1660,7 @@
       <c r="A27">
         <v>25</v>
       </c>
-      <c r="B27" s="15" t="s">
+      <c r="B27" s="14" t="s">
         <v>118</v>
       </c>
       <c r="C27" s="2">
@@ -1659,7 +1699,7 @@
       <c r="A29">
         <v>26</v>
       </c>
-      <c r="B29" s="16" t="s">
+      <c r="B29" s="19" t="s">
         <v>121</v>
       </c>
       <c r="C29" s="2">
@@ -1671,7 +1711,7 @@
       <c r="E29" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="F29" s="17" t="s">
+      <c r="F29" s="15" t="s">
         <v>123</v>
       </c>
       <c r="G29" s="2"/>
@@ -1684,7 +1724,7 @@
       <c r="A30">
         <v>27</v>
       </c>
-      <c r="B30" s="18" t="s">
+      <c r="B30" s="20" t="s">
         <v>126</v>
       </c>
       <c r="C30" s="2">
@@ -1707,10 +1747,10 @@
       <c r="A31">
         <v>28</v>
       </c>
-      <c r="B31" s="9" t="s">
+      <c r="B31" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="C31" s="19">
+      <c r="C31" s="16">
         <v>2007</v>
       </c>
       <c r="D31" s="9" t="s">
@@ -1721,10 +1761,10 @@
       <c r="A32">
         <v>29</v>
       </c>
-      <c r="B32" s="9" t="s">
+      <c r="B32" s="18" t="s">
         <v>130</v>
       </c>
-      <c r="C32" s="19">
+      <c r="C32" s="16">
         <v>2017</v>
       </c>
       <c r="D32" s="9" t="s">
@@ -1735,10 +1775,10 @@
       <c r="A33">
         <v>30</v>
       </c>
-      <c r="B33" s="15" t="s">
+      <c r="B33" s="14" t="s">
         <v>133</v>
       </c>
-      <c r="C33" s="19">
+      <c r="C33" s="16">
         <v>2013</v>
       </c>
       <c r="D33" s="9" t="s">

</xml_diff>